<commit_message>
Bug fix for Ticket #5: Allow escaping of double-quote characters in attribute values (backslashes are now escaped also).
</commit_message>
<xml_diff>
--- a/jett-core/templates/TagParserTests.xlsx
+++ b/jett-core/templates/TagParserTests.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>&lt;: attr1="blah"/&gt;</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>&lt;/custom:tag&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:escape doublequote="Embedded \"double-quotes\"" backslash="Embedded \\backslash"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
@@ -475,6 +478,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>